<commit_message>
Data scraper is done barring any enhancements that get thought of... or bugs that come up. Will begin work on csv file writer and webscraper next.
</commit_message>
<xml_diff>
--- a/Docs/CarStatsTargetData.xlsx
+++ b/Docs/CarStatsTargetData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Category</t>
   </si>
@@ -22,7 +22,10 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Values</t>
+    <t>Target Values</t>
+  </si>
+  <si>
+    <t>Output Values</t>
   </si>
   <si>
     <t>Vehicle</t>
@@ -34,10 +37,19 @@
     <t>Brand</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>Model</t>
   </si>
   <si>
+    <t>Trim</t>
+  </si>
+  <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
   <si>
     <t>Price</t>
@@ -49,6 +61,9 @@
     <t>(Filter by capital letters)</t>
   </si>
   <si>
+    <t>FWD/RWD/AWD/4WD</t>
+  </si>
+  <si>
     <t>Engine</t>
   </si>
   <si>
@@ -58,19 +73,28 @@
     <t>Engine Type</t>
   </si>
   <si>
-    <t>"Electric" or "\w-?\d+"</t>
+    <t>"\w-?\d+" or "Gas/Electric \w-?\d+" or "Electric"</t>
   </si>
   <si>
-    <t>Turbo</t>
+    <t>"\w-?\d+"/Electric</t>
   </si>
   <si>
-    <t>(Twin)Turbo</t>
+    <t>Turbos</t>
+  </si>
+  <si>
+    <t>(Twin|Intercooled) Turbo</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
   </si>
   <si>
     <t>Fuel Type</t>
   </si>
   <si>
     <t>Gas/Regular(Unleaded)/Premium(Unleaded)/Electric</t>
+  </si>
+  <si>
+    <t>Gas/Premium/Regular/Electric/Hybrid</t>
   </si>
   <si>
     <t>Displacement (liters/cubic inches)</t>
@@ -80,6 +104,9 @@
   </si>
   <si>
     <t>.split("/")[0]</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
   <si>
     <t>Maximum Horsepower @ RPM</t>
@@ -127,19 +154,19 @@
     <t>MPG (combined)</t>
   </si>
   <si>
-    <t>Extract only digits from each section. Some entries my contain "(Est)"</t>
+    <t>.split("/")[0].split(" ")[0]</t>
   </si>
   <si>
     <t>MPG (city)</t>
   </si>
   <si>
-    <t>.split("/")[1]</t>
+    <t>.split("/")[1].split(" ")[0]</t>
   </si>
   <si>
     <t>MPG (highway)</t>
   </si>
   <si>
-    <t>.split("/")[2]</t>
+    <t>.split("/")[2].split(" ")[0]</t>
   </si>
   <si>
     <t>EPA Fuel Economy Equivalent (for hybrid and electric vehicles), combined/city/highway (MPGe)</t>
@@ -197,6 +224,18 @@
   </si>
   <si>
     <t>Trunk Space</t>
+  </si>
+  <si>
+    <t>Steering</t>
+  </si>
+  <si>
+    <t>Turning Diameter / Radius, curb to curb (feet)</t>
+  </si>
+  <si>
+    <t>Turning Radius (ft.)</t>
+  </si>
+  <si>
+    <t>/2</t>
   </si>
   <si>
     <t>Weight</t>
@@ -262,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -278,11 +317,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,8 +546,8 @@
     <col customWidth="1" min="1" max="1" width="22.13"/>
     <col customWidth="1" min="2" max="2" width="42.38"/>
     <col customWidth="1" min="3" max="3" width="23.88"/>
-    <col customWidth="1" min="4" max="4" width="48.88"/>
-    <col customWidth="1" min="5" max="5" width="25.25"/>
+    <col customWidth="1" min="4" max="4" width="50.88"/>
+    <col customWidth="1" min="5" max="5" width="36.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -521,7 +563,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -547,18 +591,20 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -582,10 +628,12 @@
     </row>
     <row r="3">
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -611,10 +659,12 @@
     </row>
     <row r="4">
       <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -639,14 +689,13 @@
       <c r="AA4" s="4"/>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -672,15 +721,15 @@
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -705,11 +754,8 @@
       <c r="AA6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -717,7 +763,9 @@
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -742,13 +790,21 @@
       <c r="AA7" s="4"/>
     </row>
     <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -774,12 +830,14 @@
     </row>
     <row r="9">
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -804,16 +862,15 @@
       <c r="AA9" s="4"/>
     </row>
     <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -839,15 +896,17 @@
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -872,13 +931,18 @@
       <c r="AA11" s="4"/>
     </row>
     <row r="12">
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -903,16 +967,15 @@
       <c r="AA12" s="4"/>
     </row>
     <row r="13">
-      <c r="B13" s="3" t="s">
-        <v>28</v>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
+      <c r="D13" s="6" t="s">
+        <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>25</v>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -937,13 +1000,18 @@
       <c r="AA13" s="4"/>
     </row>
     <row r="14">
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -968,17 +1036,15 @@
       <c r="AA14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>30</v>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
+      <c r="D15" s="6" t="s">
+        <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>32</v>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1003,16 +1069,19 @@
       <c r="AA15" s="4"/>
     </row>
     <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1037,18 +1106,17 @@
       <c r="AA16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="6" t="s">
-        <v>36</v>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>38</v>
+      <c r="E17" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1074,11 +1142,18 @@
       <c r="AA17" s="4"/>
     </row>
     <row r="18">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1105,10 +1180,13 @@
     </row>
     <row r="19">
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1134,14 +1212,14 @@
       <c r="AA19" s="4"/>
     </row>
     <row r="20">
-      <c r="B20" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1167,11 +1245,17 @@
       <c r="AA20" s="4"/>
     </row>
     <row r="21">
+      <c r="B21" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1198,10 +1282,13 @@
     </row>
     <row r="22">
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1227,14 +1314,15 @@
       <c r="AA22" s="4"/>
     </row>
     <row r="23">
-      <c r="B23" s="3" t="s">
-        <v>44</v>
+      <c r="C23" s="3" t="s">
+        <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>45</v>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1259,17 +1347,16 @@
       <c r="AA23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1294,14 +1381,19 @@
       <c r="AA24" s="4"/>
     </row>
     <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1327,13 +1419,15 @@
     </row>
     <row r="26">
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1359,13 +1453,15 @@
     </row>
     <row r="27">
       <c r="B27" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1390,17 +1486,16 @@
       <c r="AA27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1425,14 +1520,19 @@
       <c r="AA28" s="4"/>
     </row>
     <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="B29" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1458,13 +1558,15 @@
     </row>
     <row r="30">
       <c r="B30" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -1489,17 +1591,16 @@
       <c r="AA30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -1524,14 +1625,21 @@
       <c r="AA31" s="4"/>
     </row>
     <row r="32">
-      <c r="B32" s="3" t="s">
-        <v>64</v>
+      <c r="A32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1556,11 +1664,19 @@
       <c r="AA32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -1585,11 +1701,16 @@
       <c r="AA33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -29598,22 +29719,79 @@
       <c r="Z999" s="4"/>
       <c r="AA999" s="4"/>
     </row>
+    <row r="1000">
+      <c r="A1000" s="4"/>
+      <c r="B1000" s="4"/>
+      <c r="C1000" s="4"/>
+      <c r="D1000" s="4"/>
+      <c r="E1000" s="4"/>
+      <c r="F1000" s="4"/>
+      <c r="G1000" s="4"/>
+      <c r="H1000" s="4"/>
+      <c r="I1000" s="4"/>
+      <c r="J1000" s="4"/>
+      <c r="K1000" s="4"/>
+      <c r="L1000" s="4"/>
+      <c r="M1000" s="4"/>
+      <c r="N1000" s="4"/>
+      <c r="O1000" s="4"/>
+      <c r="P1000" s="4"/>
+      <c r="Q1000" s="4"/>
+      <c r="R1000" s="4"/>
+      <c r="S1000" s="4"/>
+      <c r="T1000" s="4"/>
+      <c r="U1000" s="4"/>
+      <c r="V1000" s="4"/>
+      <c r="W1000" s="4"/>
+      <c r="X1000" s="4"/>
+      <c r="Y1000" s="4"/>
+      <c r="Z1000" s="4"/>
+      <c r="AA1000" s="4"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="4"/>
+      <c r="B1001" s="4"/>
+      <c r="C1001" s="4"/>
+      <c r="D1001" s="4"/>
+      <c r="E1001" s="4"/>
+      <c r="F1001" s="4"/>
+      <c r="G1001" s="4"/>
+      <c r="H1001" s="4"/>
+      <c r="I1001" s="4"/>
+      <c r="J1001" s="4"/>
+      <c r="K1001" s="4"/>
+      <c r="L1001" s="4"/>
+      <c r="M1001" s="4"/>
+      <c r="N1001" s="4"/>
+      <c r="O1001" s="4"/>
+      <c r="P1001" s="4"/>
+      <c r="Q1001" s="4"/>
+      <c r="R1001" s="4"/>
+      <c r="S1001" s="4"/>
+      <c r="T1001" s="4"/>
+      <c r="U1001" s="4"/>
+      <c r="V1001" s="4"/>
+      <c r="W1001" s="4"/>
+      <c r="X1001" s="4"/>
+      <c r="Y1001" s="4"/>
+      <c r="Z1001" s="4"/>
+      <c r="AA1001" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B20:B22"/>
+  <mergeCells count="13">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A24"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
File writer works. Added a url column to data.
</commit_message>
<xml_diff>
--- a/Docs/CarStatsTargetData.xlsx
+++ b/Docs/CarStatsTargetData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>Category</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Towing Capacity</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -1735,11 +1738,17 @@
       <c r="AA34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -29781,7 +29790,7 @@
   <mergeCells count="13">
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A18:A24"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A33:A34"/>
@@ -29791,7 +29800,7 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B21:B23"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>